<commit_message>
GGWP T:N/A S0 - Cambios en gestión de configuración
</commit_message>
<xml_diff>
--- a/proyecto/documentos/Tabla gestión de configuración.xlsx
+++ b/proyecto/documentos/Tabla gestión de configuración.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsmaFunes\Documents\Repositories\GitHub\GGWP\proyecto\documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ifunes\Documents\GitHub\GGWP\proyecto\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982A052D-355C-4426-8D83-2266CA09F9FA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Nombre del ítem de configuración</t>
   </si>
@@ -75,9 +76,6 @@
     <t>Daily Meeting</t>
   </si>
   <si>
-    <t>dd/mm/aaaa DailyMeeting</t>
-  </si>
-  <si>
     <t>/PROYECTO/sprint #/daily meetings</t>
   </si>
   <si>
@@ -99,12 +97,6 @@
     <t>Significado</t>
   </si>
   <si>
-    <t>&lt;dd/mm/aaaa&gt;</t>
-  </si>
-  <si>
-    <t>Fecha en formato día/mes/año</t>
-  </si>
-  <si>
     <t>&lt;#.#&gt;</t>
   </si>
   <si>
@@ -126,19 +118,61 @@
     <t>Sprint</t>
   </si>
   <si>
-    <t>GGWP-[USN] S# - [NombreUserStory]</t>
-  </si>
-  <si>
     <t>Retrospectiva S#</t>
   </si>
   <si>
     <t>SprintBacklog S#</t>
+  </si>
+  <si>
+    <t>GGWP-[USN] [Sprint] - [NombreUserStory]</t>
+  </si>
+  <si>
+    <t>Ejemplo</t>
+  </si>
+  <si>
+    <t>&lt;ddmmaaaa&gt;</t>
+  </si>
+  <si>
+    <t>aaaammdd DailyMeeting</t>
+  </si>
+  <si>
+    <t>Fecha en formato año/mes/día</t>
+  </si>
+  <si>
+    <t>V#.# S#</t>
+  </si>
+  <si>
+    <t>GGWP-24 V1.1 S3 - Consultar Socio</t>
+  </si>
+  <si>
+    <t>ProductBacklog v1.2</t>
+  </si>
+  <si>
+    <t>GGWP-DEV v2.3</t>
+  </si>
+  <si>
+    <t>001 - Generar Navegación</t>
+  </si>
+  <si>
+    <t>Metrica - Burndown Chart</t>
+  </si>
+  <si>
+    <t>03082018 Daily Meeting</t>
+  </si>
+  <si>
+    <t>Retrospectiva v1.1 S3</t>
+  </si>
+  <si>
+    <t>Sprint Backlog v1.1 S3</t>
+  </si>
+  <si>
+    <t>V1.1 S3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -198,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -221,16 +255,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -242,13 +314,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -530,14 +611,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -545,6 +626,7 @@
     <col min="1" max="1" width="31.7109375" customWidth="1"/>
     <col min="2" max="2" width="34.5703125" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -557,379 +639,397 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="D1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="D2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="D3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="D4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="D5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="D6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="D8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="B16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="B17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+      <c r="B18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+      <c r="B19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>